<commit_message>
Atualização do controlo de progresso
</commit_message>
<xml_diff>
--- a/Projeto/BDII_ControloProgressoProjecto_v2.xlsx
+++ b/Projeto/BDII_ControloProgressoProjecto_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\BD2\restauro_de_veiculos\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\BD2\restauro_de_veiculos\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F33D6C-B8B7-44BD-B22A-0DD2FBA4E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214A14F-BE9B-4260-B4E6-AB1F4C9DBB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking Projecto" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -392,6 +392,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -751,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -876,6 +884,7 @@
     <xf numFmtId="164" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1283,22 +1292,22 @@
   </sheetPr>
   <dimension ref="A1:AMJ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="1" customWidth="1"/>
     <col min="6" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="1024" width="9.140625" style="1"/>
+    <col min="8" max="1024" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1306,13 +1315,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45212</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -1352,7 +1361,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>19</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
@@ -1458,7 +1467,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="98" t="s">
         <v>23</v>
       </c>
@@ -1481,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="102" t="s">
         <v>25</v>
       </c>
@@ -1504,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="102" t="s">
         <v>27</v>
       </c>
@@ -1527,7 +1536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="80" t="s">
         <v>29</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
         <v>31</v>
       </c>
@@ -1573,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
         <v>33</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="73" t="s">
         <v>35</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>19</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
@@ -1653,7 +1662,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="66" t="s">
         <v>40</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="73" t="s">
         <v>41</v>
       </c>
@@ -1699,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="102" t="s">
         <v>42</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="102" t="s">
         <v>44</v>
       </c>
@@ -1737,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="102" t="s">
         <v>46</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="66" t="s">
         <v>50</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="80" t="s">
         <v>51</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="66" t="s">
         <v>50</v>
       </c>
@@ -1830,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="80" t="s">
         <v>51</v>
       </c>
@@ -1849,15 +1858,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="73" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
+      <c r="C31" s="75">
+        <v>45505</v>
+      </c>
+      <c r="D31" s="76">
+        <v>45512</v>
+      </c>
       <c r="E31" s="77" t="s">
         <v>85</v>
       </c>
@@ -1868,14 +1881,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="73" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="75"/>
+      <c r="C32" s="75">
+        <v>45515</v>
+      </c>
       <c r="D32" s="76"/>
       <c r="E32" s="77" t="s">
         <v>85</v>
@@ -1887,14 +1902,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="73" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="75"/>
+      <c r="C33" s="112"/>
       <c r="D33" s="76"/>
       <c r="E33" s="77" t="s">
         <v>85</v>
@@ -1906,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="64" t="s">
         <v>51</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="85" t="s">
         <v>51</v>
       </c>
@@ -1944,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="66" t="s">
         <v>52</v>
       </c>
@@ -1963,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="80" t="s">
         <v>51</v>
       </c>
@@ -1982,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="73" t="s">
         <v>50</v>
       </c>
@@ -2001,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="78" t="s">
         <v>51</v>
       </c>
@@ -2020,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="71" t="s">
         <v>51</v>
       </c>
@@ -2039,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="87" t="s">
         <v>51</v>
       </c>
@@ -2058,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="87" t="s">
         <v>51</v>
       </c>
@@ -2077,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="87" t="s">
         <v>51</v>
       </c>
@@ -2096,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="87" t="s">
         <v>51</v>
       </c>
@@ -2115,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="107" t="s">
         <v>51</v>
       </c>
@@ -2134,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="85" t="s">
         <v>51</v>
       </c>
@@ -2153,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="30" t="s">
         <v>53</v>
       </c>
@@ -2174,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>55</v>
       </c>
@@ -2191,7 +2206,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="29" t="s">
         <v>59</v>
       </c>
@@ -2227,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="39" t="s">
         <v>61</v>
       </c>
@@ -2244,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="42" t="s">
         <v>63</v>
       </c>
@@ -2261,7 +2276,7 @@
       <c r="F56" s="43"/>
       <c r="G56" s="42"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="46" t="s">
         <v>66</v>
       </c>
@@ -2280,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="53" t="s">
         <v>68</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="53" t="s">
         <v>70</v>
       </c>
@@ -2318,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="53" t="s">
         <v>72</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="53" t="s">
         <v>74</v>
       </c>
@@ -2356,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="53" t="s">
         <v>76</v>
       </c>
@@ -2375,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="53" t="s">
         <v>78</v>
       </c>
@@ -2394,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="56" t="s">
         <v>80</v>
       </c>

</xml_diff>